<commit_message>
Resuelto cambio de limites
</commit_message>
<xml_diff>
--- a/Reserva_entrada.xlsx
+++ b/Reserva_entrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbru\Desktop\psie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1A2F59-9468-4596-A54A-CB97A63EDDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE107594-8467-443C-86EE-19643D85A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,7 +943,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
resuelto el tema de los limites
</commit_message>
<xml_diff>
--- a/Reserva_entrada.xlsx
+++ b/Reserva_entrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbru\Desktop\psie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE107594-8467-443C-86EE-19643D85A957}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7264642-FB30-402C-8B49-92404E04ABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -943,7 +943,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Solucionado el tema del cambio del limte
</commit_message>
<xml_diff>
--- a/Reserva_entrada.xlsx
+++ b/Reserva_entrada.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbru\Desktop\psie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7264642-FB30-402C-8B49-92404E04ABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC4FD2F-424D-4015-982F-1480A79D80A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="1290" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parametros" sheetId="4" r:id="rId1"/>
@@ -943,7 +943,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,7 +988,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="18" t="s">
         <v>15</v>
@@ -1080,6 +1080,7 @@
     <mergeCell ref="E9:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Tratando de arreglar el formato
</commit_message>
<xml_diff>
--- a/Reserva_entrada.xlsx
+++ b/Reserva_entrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbru\Desktop\psie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{219CC5D6-3BB0-4FF9-9879-D1206C681A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4162CA-EE1B-42C8-A59B-9229B4451972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -650,6 +650,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -668,7 +669,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -952,7 +952,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,10 +973,10 @@
       <c r="B1" s="10">
         <v>15</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
@@ -999,10 +999,10 @@
       <c r="B3" s="12">
         <v>0</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1011,48 +1011,48 @@
         <v>17</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="22"/>
+        <v>1</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="E4" s="23"/>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D5" s="18"/>
-      <c r="E5" s="22" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="23" t="s">
         <v>41</v>
       </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D6" s="18"/>
-      <c r="E6" s="22"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D7" s="17" t="s">
+      <c r="D7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="23" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="18"/>
-      <c r="E8" s="22"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="18"/>
-      <c r="E9" s="22" t="s">
+      <c r="D9" s="19"/>
+      <c r="E9" s="23" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D10" s="18"/>
-      <c r="E10" s="22"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="23"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="D11" s="17" t="s">
+      <c r="D11" s="18" t="s">
         <v>45</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -1060,14 +1060,14 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C12" s="23"/>
-      <c r="D12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="19"/>
+      <c r="D13" s="20"/>
       <c r="E13" s="6" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
Revisado en su totalidad
</commit_message>
<xml_diff>
--- a/Reserva_entrada.xlsx
+++ b/Reserva_entrada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcbru\Desktop\psie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA519FFF-A98D-4C89-AE22-D126241EED60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9702ADE1-3706-4C1E-A16E-5A2A6AE66902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -952,7 +952,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +997,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>15</v>
@@ -1011,7 +1011,7 @@
         <v>17</v>
       </c>
       <c r="B4" s="14">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" s="23"/>

</xml_diff>